<commit_message>
Individual .csv's for each process
I am dividing up the work across 4 processes and each process has a .csv file.
</commit_message>
<xml_diff>
--- a/TheGrail.xlsx
+++ b/TheGrail.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattmawson/Desktop/Euler800/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5EF4F694-E95E-2543-9B85-BC471263ABD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1987E5-F5FF-7942-8DEC-5A9482D86EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{6DC91989-0AC4-9E40-93D4-F650661E752D}"/>
+    <workbookView xWindow="300" yWindow="0" windowWidth="28040" windowHeight="17440" xr2:uid="{6DC91989-0AC4-9E40-93D4-F650661E752D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8C09F7C-5161-7B48-AD89-43AA0042D672}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -394,13 +394,17 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>2</v>
       </c>
       <c r="B1" s="1">
         <v>1013277</v>
       </c>
+      <c r="C1" t="str">
+        <f>"-Wolfram"</f>
+        <v>-Wolfram</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>